<commit_message>
Run csv export tool and add 3.1 files
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-1.4.2-us - AEO Update\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B894A-F356-4233-B257-22D3D9ACBC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="20100" windowHeight="7410" activeTab="1"/>
+    <workbookView xWindow="5310" yWindow="1590" windowWidth="21660" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -238,13 +249,16 @@
     <t>2018.............................................................................     .</t>
   </si>
   <si>
-    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201812.pdf</t>
+    <t>2019.............................................................................     .</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -403,6 +417,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -438,6 +469,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,12 +661,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -637,7 +683,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,7 +693,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +723,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -685,12 +731,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1228,7 +1272,7 @@
         <v>4.2</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G56" si="0">$D$50/D29</f>
+        <f t="shared" ref="G29:G57" si="0">$D$50/D29</f>
         <v>1.6857121879588841</v>
       </c>
       <c r="M29" s="1"/>
@@ -1963,6 +2007,30 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>254.41200000000001</v>
+      </c>
+      <c r="C57">
+        <v>256.90300000000002</v>
+      </c>
+      <c r="D57">
+        <v>255.65700000000001</v>
+      </c>
+      <c r="E57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F57">
+        <v>1.8</v>
+      </c>
+      <c r="G57" s="6">
+        <f t="shared" si="0"/>
+        <v>0.89805481563188172</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>